<commit_message>
Adding item outlines to Eagle as part of DFM issues
</commit_message>
<xml_diff>
--- a/base/BoM/CSv2.0_BOM_Eagle_formatted.xlsx
+++ b/base/BoM/CSv2.0_BOM_Eagle_formatted.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work-reese/hardware/commonsense/cs-hardware/base/BoM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F20903-C4DB-9F49-A011-87FE667219DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3CFCD1-4C3C-B240-8282-4750FC5C574F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{CF684D7E-97D6-5A41-916A-A4D95D53D270}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{DF2471A0-007B-DC4F-81CA-EFE688E6BD07}" name="cs_v2" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/work-reese/hardware/commonsense/cs-hardware/base/BoM/cs_v2.csv" semicolon="1">
+    <textPr sourceFile="/Users/work-reese/hardware/commonsense/cs-hardware/base/BoM/cs_v2.csv" semicolon="1">
       <textFields count="39">
         <textField/>
         <textField/>
@@ -127,9 +127,6 @@
     <t>JST 2-Pin Connector</t>
   </si>
   <si>
-    <t xml:space="preserve">SM02B-SRSS-TB(LF)(SN) </t>
-  </si>
-  <si>
     <t>SWITCH_SPST_SMD_A</t>
   </si>
   <si>
@@ -626,6 +623,9 @@
   </si>
   <si>
     <t>Test pad</t>
+  </si>
+  <si>
+    <t>S2B-PH-SM4-TB(LF)(SN)</t>
   </si>
 </sst>
 </file>
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C92848B-B750-A949-8386-EC656E33A1D6}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1049,7 +1049,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1057,16 +1057,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1074,28 +1074,28 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
       </c>
       <c r="H4" s="1">
         <v>0.1</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1106,16 +1106,16 @@
         <v>0.51</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="H5" s="1">
         <v>0.01</v>
@@ -1129,16 +1129,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
         <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
       </c>
       <c r="H6" s="1">
         <v>0.01</v>
@@ -1152,16 +1152,16 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
         <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
       </c>
       <c r="H7" s="2">
         <v>5.0000000000000001E-3</v>
@@ -1172,28 +1172,28 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>35</v>
-      </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="1">
         <v>0.1</v>
       </c>
       <c r="J8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1201,19 +1201,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
         <v>39</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
       </c>
       <c r="H9" s="1">
         <v>0.05</v>
@@ -1224,19 +1224,19 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
         <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>43</v>
       </c>
       <c r="H10" s="1">
         <v>0.05</v>
@@ -1247,28 +1247,28 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
         <v>45</v>
       </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>46</v>
-      </c>
       <c r="G11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="1">
         <v>0.1</v>
       </c>
       <c r="J11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1276,28 +1276,28 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
         <v>47</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>48</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
         <v>49</v>
       </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>50</v>
-      </c>
-      <c r="G12" t="s">
-        <v>51</v>
       </c>
       <c r="H12" s="1">
         <v>0.1</v>
       </c>
       <c r="J12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1305,28 +1305,28 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
         <v>52</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
         <v>53</v>
       </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" t="s">
-        <v>54</v>
-      </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="1">
         <v>0.1</v>
       </c>
       <c r="J13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1334,16 +1334,16 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>57</v>
-      </c>
-      <c r="F14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1351,19 +1351,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
         <v>59</v>
       </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
         <v>60</v>
-      </c>
-      <c r="E15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" t="s">
-        <v>61</v>
       </c>
       <c r="H15" s="2">
         <v>5.0000000000000001E-3</v>
@@ -1374,19 +1374,19 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
         <v>62</v>
-      </c>
-      <c r="E16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" t="s">
-        <v>63</v>
       </c>
       <c r="H16" s="1">
         <v>0.05</v>
@@ -1397,28 +1397,28 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
         <v>64</v>
       </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
         <v>65</v>
       </c>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" t="s">
-        <v>66</v>
-      </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H17" s="1">
         <v>0.1</v>
       </c>
       <c r="J17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1426,28 +1426,28 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" t="s">
         <v>67</v>
       </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" t="s">
-        <v>68</v>
-      </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H18" s="1">
         <v>0.1</v>
       </c>
       <c r="J18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1455,16 +1455,16 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
         <v>69</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>70</v>
-      </c>
-      <c r="F19" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1472,28 +1472,28 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s">
         <v>72</v>
       </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
         <v>73</v>
       </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" t="s">
-        <v>74</v>
-      </c>
       <c r="G20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H20" s="1">
         <v>0.1</v>
       </c>
       <c r="J20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1504,16 +1504,16 @@
         <v>330</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
         <v>75</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" t="s">
-        <v>76</v>
       </c>
       <c r="H21" s="1">
         <v>0.05</v>
@@ -1527,16 +1527,16 @@
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
         <v>77</v>
-      </c>
-      <c r="E22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" t="s">
-        <v>78</v>
       </c>
       <c r="H22" s="1">
         <v>0.05</v>
@@ -1547,19 +1547,19 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
         <v>79</v>
       </c>
-      <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
         <v>80</v>
-      </c>
-      <c r="E23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" t="s">
-        <v>81</v>
       </c>
       <c r="H23" s="1">
         <v>0.05</v>
@@ -1570,28 +1570,28 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" t="s">
         <v>82</v>
       </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" t="s">
         <v>83</v>
       </c>
-      <c r="E24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" t="s">
-        <v>84</v>
-      </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H24" s="1">
         <v>0.1</v>
       </c>
       <c r="J24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1599,28 +1599,28 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
         <v>85</v>
       </c>
-      <c r="C25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
         <v>86</v>
       </c>
-      <c r="E25" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" t="s">
-        <v>87</v>
-      </c>
       <c r="G25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H25" s="1">
         <v>0.1</v>
       </c>
       <c r="J25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1631,16 +1631,16 @@
         <v>590</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
         <v>88</v>
-      </c>
-      <c r="E26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" t="s">
-        <v>89</v>
       </c>
       <c r="H26" s="1">
         <v>0.01</v>
@@ -1651,28 +1651,28 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
         <v>90</v>
       </c>
-      <c r="C27" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" t="s">
         <v>91</v>
       </c>
-      <c r="E27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" t="s">
-        <v>92</v>
-      </c>
       <c r="G27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H27" s="1">
         <v>0.1</v>
       </c>
       <c r="J27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1680,19 +1680,19 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s">
         <v>93</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>94</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>95</v>
       </c>
-      <c r="E28" t="s">
-        <v>96</v>
-      </c>
       <c r="F28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -1700,19 +1700,19 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" t="s">
         <v>97</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>98</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>99</v>
       </c>
-      <c r="E29" t="s">
-        <v>100</v>
-      </c>
       <c r="F29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -1720,19 +1720,19 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" t="s">
         <v>101</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>102</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>103</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>104</v>
-      </c>
-      <c r="F30" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -1740,19 +1740,19 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" t="s">
         <v>106</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>107</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>108</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>109</v>
-      </c>
-      <c r="F31" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -1760,19 +1760,19 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" t="s">
         <v>111</v>
       </c>
-      <c r="C32" t="s">
-        <v>111</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>112</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>113</v>
-      </c>
-      <c r="F32" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1780,19 +1780,19 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" t="s">
         <v>115</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>116</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>117</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>118</v>
-      </c>
-      <c r="F33" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1800,19 +1800,19 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" t="s">
         <v>120</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>121</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>122</v>
       </c>
-      <c r="E34" t="s">
-        <v>123</v>
-      </c>
       <c r="F34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1820,19 +1820,19 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" t="s">
         <v>124</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>125</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>126</v>
       </c>
-      <c r="E35" t="s">
-        <v>127</v>
-      </c>
       <c r="F35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1840,19 +1840,19 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" t="s">
         <v>128</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>129</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>130</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>131</v>
-      </c>
-      <c r="F36" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1860,19 +1860,19 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" t="s">
         <v>133</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>134</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>135</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>136</v>
-      </c>
-      <c r="F37" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1880,16 +1880,16 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" t="s">
         <v>138</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>139</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>140</v>
-      </c>
-      <c r="E38" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1897,16 +1897,16 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" t="s">
         <v>142</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>143</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>144</v>
-      </c>
-      <c r="E39" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1914,16 +1914,16 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" t="s">
         <v>146</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>147</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>148</v>
-      </c>
-      <c r="E40" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1931,16 +1931,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" t="s">
         <v>150</v>
       </c>
-      <c r="C41" t="s">
-        <v>150</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="F41" t="s">
         <v>151</v>
-      </c>
-      <c r="F41" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1948,19 +1948,19 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" t="s">
+        <v>152</v>
+      </c>
+      <c r="D42" t="s">
         <v>153</v>
       </c>
-      <c r="C42" t="s">
-        <v>153</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>154</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>155</v>
-      </c>
-      <c r="F42" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1968,19 +1968,19 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" t="s">
         <v>157</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>158</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>159</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>160</v>
-      </c>
-      <c r="F43" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1988,19 +1988,19 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
+        <v>161</v>
+      </c>
+      <c r="C44" t="s">
         <v>162</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>163</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>164</v>
       </c>
-      <c r="E44" t="s">
-        <v>165</v>
-      </c>
       <c r="F44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2008,19 +2008,19 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" t="s">
         <v>166</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>167</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>168</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>169</v>
-      </c>
-      <c r="F45" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2028,19 +2028,19 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
+        <v>170</v>
+      </c>
+      <c r="C46" t="s">
         <v>171</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>172</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>173</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>174</v>
-      </c>
-      <c r="F46" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2048,16 +2048,16 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" t="s">
         <v>176</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>177</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>178</v>
-      </c>
-      <c r="E47" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>